<commit_message>
Az 1.4es feladathoz tartozó lista bohóckodás javításra került
</commit_message>
<xml_diff>
--- a/LKYEOR_python_adat.xlsx
+++ b/LKYEOR_python_adat.xlsx
@@ -472,22 +472,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>109.6667579908676</v>
+        <v>107.1061711711712</v>
       </c>
       <c r="C2" t="n">
-        <v>89.688</v>
+        <v>89.21600000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>105.2044368266405</v>
+        <v>106.7146138807429</v>
       </c>
       <c r="E2" t="n">
-        <v>110.728</v>
+        <v>118.5287924528302</v>
       </c>
       <c r="F2" t="n">
-        <v>94.21091743119266</v>
+        <v>95.18405063291139</v>
       </c>
       <c r="G2" t="n">
-        <v>101.8996224497401</v>
+        <v>103.3499256275311</v>
       </c>
     </row>
     <row r="3">
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50.47488584474886</v>
+        <v>52.2972972972973</v>
       </c>
       <c r="C3" t="n">
-        <v>16.8</v>
+        <v>15.2</v>
       </c>
       <c r="D3" t="n">
-        <v>45.26836434867776</v>
+        <v>45.6236559139785</v>
       </c>
       <c r="E3" t="n">
-        <v>60.14545454545455</v>
+        <v>59.81132075471698</v>
       </c>
       <c r="F3" t="n">
-        <v>7.28</v>
+        <v>6.729789029535866</v>
       </c>
       <c r="G3" t="n">
-        <v>35.99374094777623</v>
+        <v>35.93241259910572</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>30.34794520547945</v>
+        <v>30.7972972972973</v>
       </c>
       <c r="C4" t="n">
-        <v>24.79</v>
+        <v>24.46</v>
       </c>
       <c r="D4" t="n">
-        <v>30.11057786483839</v>
+        <v>30.37429130009775</v>
       </c>
       <c r="E4" t="n">
-        <v>30.30072727272728</v>
+        <v>30.18339622641509</v>
       </c>
       <c r="F4" t="n">
-        <v>19.97568807339449</v>
+        <v>19.88354430379747</v>
       </c>
       <c r="G4" t="n">
-        <v>27.10498768328792</v>
+        <v>27.13970582552152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2.4es feladatban nem csökkenő sorrendben helyeztem a hisztogrammot
</commit_message>
<xml_diff>
--- a/LKYEOR_python_adat.xlsx
+++ b/LKYEOR_python_adat.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="LKYEOR" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LKYEOR" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>